<commit_message>
some small changes to prepare to give this version to Jenny
Former-commit-id: b186cdea44e4242485d26b73a90fd47cd8d069ea
</commit_message>
<xml_diff>
--- a/RCP4.5/RCP45_85_GCM_names.xlsx
+++ b/RCP4.5/RCP45_85_GCM_names.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahfletcher/Dropbox (MIT)/Mwache Climate Project/RCP4.5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahfletcher/Dropbox (MIT)/Mombasa_Climate/RCP4.5/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="2720" windowWidth="25360" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="440" windowWidth="37360" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="30">
   <si>
     <t>ACCESS1-0_run1</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>RCP85</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>RCP8.5 In paper</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>In Paper</t>
   </si>
 </sst>
 </file>
@@ -153,17 +165,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -498,15 +514,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G17:G18"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
@@ -588,70 +624,289 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
+      </c>
+      <c r="N3">
+        <v>13</v>
+      </c>
+      <c r="O3">
+        <v>14</v>
+      </c>
+      <c r="P3">
+        <v>15</v>
+      </c>
+      <c r="Q3">
+        <v>16</v>
+      </c>
+      <c r="R3">
+        <v>17</v>
+      </c>
+      <c r="S3">
+        <v>18</v>
+      </c>
+      <c r="T3">
+        <v>19</v>
+      </c>
+      <c r="U3">
+        <v>20</v>
+      </c>
+      <c r="V3">
+        <v>21</v>
+      </c>
+      <c r="W3">
+        <v>22</v>
+      </c>
+      <c r="X3">
+        <v>23</v>
+      </c>
+      <c r="Y3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I5" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J5" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K5" t="s">
         <v>9</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L5" t="s">
         <v>10</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M5" t="s">
         <v>11</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N5" t="s">
         <v>14</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O5" t="s">
         <v>15</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P5" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q5" t="s">
         <v>17</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R5" t="s">
         <v>18</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S5" t="s">
         <v>19</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T5" t="s">
         <v>20</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U5" t="s">
         <v>22</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V5" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6" t="s">
+        <v>26</v>
+      </c>
+      <c r="U6" t="s">
+        <v>26</v>
+      </c>
+      <c r="V6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>